<commit_message>
Graph API adjustments for client accounts
</commit_message>
<xml_diff>
--- a/Programming/User Directory/Which Processor does which Zone.xlsx
+++ b/Programming/User Directory/Which Processor does which Zone.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marci\Dropbox (Smartcomm Ltd)\PC\Documents\Smartcomm\Projects\Hammersmith-and-Fulham\Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marci\Documents\Smartcomm\Projects\Hammersmith-and-Fulham\Programming\User Directory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80A4DB85-AB40-4519-8CBE-A6D6753AF1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6444887E-9DB8-40D7-A867-9A064E18E162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Processor Location</t>
   </si>
@@ -37,81 +36,30 @@
     <t>Zones Controlled by Processor</t>
   </si>
   <si>
-    <t>Small Hall</t>
-  </si>
-  <si>
     <t>Prcessor Model</t>
   </si>
   <si>
     <t>CP4N</t>
   </si>
   <si>
-    <t>Courtyard Room 02</t>
-  </si>
-  <si>
     <t>RMC4</t>
   </si>
   <si>
     <t>Registar Waiting Area</t>
   </si>
   <si>
-    <t>Courtyard Room 01</t>
-  </si>
-  <si>
     <t>Foyer / Shared Workspace</t>
   </si>
   <si>
-    <t>Committee Room 01</t>
-  </si>
-  <si>
-    <t>Committee Room 02</t>
-  </si>
-  <si>
-    <t>Committee Room 03</t>
-  </si>
-  <si>
-    <t>Committee Room 04</t>
-  </si>
-  <si>
-    <t>Assembly Hall Rack</t>
-  </si>
-  <si>
-    <t>Assembly Hall</t>
-  </si>
-  <si>
     <t>Marble Gallery</t>
   </si>
   <si>
-    <t>Nigel Playfair Room</t>
-  </si>
-  <si>
-    <t>Courtyard Room 03</t>
-  </si>
-  <si>
-    <t>Courtyard Room 04</t>
-  </si>
-  <si>
-    <t>Courtyard Room 05</t>
-  </si>
-  <si>
     <t>Council Chamber Ante Room Rack</t>
   </si>
   <si>
     <t>Council Chamber</t>
   </si>
   <si>
-    <t>Rievrside Room</t>
-  </si>
-  <si>
-    <t>Courtyard Room 06</t>
-  </si>
-  <si>
-    <t>Courtyard Room 07</t>
-  </si>
-  <si>
-    <t>Courtyard Room 08</t>
-  </si>
-  <si>
     <t>Opposition Room &amp; Office</t>
   </si>
   <si>
@@ -127,41 +75,95 @@
     <t>Leaders Office</t>
   </si>
   <si>
-    <t>Mamber's Cabinet Room</t>
-  </si>
-  <si>
-    <t>Meeting Room 02 - Large</t>
-  </si>
-  <si>
-    <t>Meeting Room 03 - Small</t>
-  </si>
-  <si>
-    <t>Meeting Room 04 - Small</t>
-  </si>
-  <si>
-    <t>Meeting Room 01 - Large</t>
-  </si>
-  <si>
     <t>Office Collaboration</t>
   </si>
   <si>
-    <t>Member's Meeting Room 01</t>
-  </si>
-  <si>
     <t>Member's Office</t>
   </si>
   <si>
     <t>Config Files Prepared</t>
   </si>
   <si>
-    <t>Small Hall Rack</t>
+    <t>Courtyard Room 01 / Rosalind Franklin</t>
+  </si>
+  <si>
+    <t>Committee Room 01 / Meeting Room G.1</t>
+  </si>
+  <si>
+    <t>Committee Room 02 / Meeting Room G.2</t>
+  </si>
+  <si>
+    <t>Committee Room 03 / Meeting Room G.3</t>
+  </si>
+  <si>
+    <t>Committee Room 04 / Meeting Room G.4</t>
+  </si>
+  <si>
+    <t>Courtyard Room 02 / The Esther Bruce Room</t>
+  </si>
+  <si>
+    <t>Small Hall / Betty Boothroyd</t>
+  </si>
+  <si>
+    <t>Small Hall / Betty Boothroyd Rack</t>
+  </si>
+  <si>
+    <t>Assembly Hall / Playfair Hall Rack</t>
+  </si>
+  <si>
+    <t>Assembly Hall / Playfair Hall</t>
+  </si>
+  <si>
+    <t>Courtyard Room 03 / Meeting Room 1.1</t>
+  </si>
+  <si>
+    <t>Courtyard Room 04 / Meeting Room 1.2</t>
+  </si>
+  <si>
+    <t>Courtyard Room 05 / Meeting Room 1.3</t>
+  </si>
+  <si>
+    <t>Courtyard Room 06 / Meeting Room 2.1</t>
+  </si>
+  <si>
+    <t>Courtyard Room 07 / Meeting Room 2.2</t>
+  </si>
+  <si>
+    <t>Courtyard Room 08 / Meeting Room 2.3</t>
+  </si>
+  <si>
+    <t>Nigel Playfair Room / The Cartwright &amp; Aherne</t>
+  </si>
+  <si>
+    <t>Rievrside Room / The Cecilia Payne Gaposchkin Room</t>
+  </si>
+  <si>
+    <t>Meeting Room 01 / Meeting Room 5.1</t>
+  </si>
+  <si>
+    <t>Meeting Room 02 / Meeting Room 5.2</t>
+  </si>
+  <si>
+    <t>Meeting Room 03 / Meeting Room 5.3</t>
+  </si>
+  <si>
+    <t>Meeting Room 04 / Meeting Room 5.4</t>
+  </si>
+  <si>
+    <t>Members' Meeting Room 01</t>
+  </si>
+  <si>
+    <t>Members' Meeting Room 01 / Members' Meeting Room</t>
+  </si>
+  <si>
+    <t>Mamber's Cabinet Room / The Cabinet Room</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +181,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,13 +220,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -235,8 +244,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -252,11 +261,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
@@ -265,16 +274,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="2" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
     <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
-    <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
-    <cellStyle name="Bad" xfId="5" builtinId="27"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -557,7 +566,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +574,7 @@
     <col min="1" max="1" width="43.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="51.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="30.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -577,13 +586,13 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -591,26 +600,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="8" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -619,20 +628,20 @@
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="9" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E5" s="7"/>
     </row>
@@ -641,20 +650,20 @@
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E7" s="7"/>
     </row>
@@ -663,20 +672,20 @@
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
       <c r="D8" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="9" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E9" s="7"/>
     </row>
@@ -685,7 +694,7 @@
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E10" s="7"/>
     </row>
@@ -694,13 +703,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E12" s="7"/>
     </row>
@@ -709,7 +718,7 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E13" s="7"/>
     </row>
@@ -718,20 +727,20 @@
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E15" s="7"/>
     </row>
@@ -740,7 +749,7 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E16" s="7"/>
     </row>
@@ -749,7 +758,7 @@
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E17" s="7"/>
     </row>
@@ -758,13 +767,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E19" s="7"/>
     </row>
@@ -773,20 +782,20 @@
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="3" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="9" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E21" s="7"/>
     </row>
@@ -795,7 +804,7 @@
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E22" s="7"/>
     </row>
@@ -804,7 +813,7 @@
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E23" s="7"/>
     </row>
@@ -816,13 +825,13 @@
         <v>3</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E25" s="7"/>
     </row>
@@ -831,7 +840,7 @@
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="3" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E26" s="7"/>
     </row>
@@ -840,13 +849,13 @@
         <v>5</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E28" s="7"/>
     </row>
@@ -855,7 +864,7 @@
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E29" s="7"/>
     </row>
@@ -864,7 +873,7 @@
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E30" s="7"/>
     </row>
@@ -874,7 +883,7 @@
         <v>37</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>37</v>
@@ -886,20 +895,20 @@
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="3" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E33" s="7"/>
     </row>
@@ -908,46 +917,46 @@
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="E37" s="5"/>
     </row>
@@ -996,5 +1005,6 @@
     <mergeCell ref="E21:E23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>